<commit_message>
add all python files
</commit_message>
<xml_diff>
--- a/Codebook for Error Check.xlsx
+++ b/Codebook for Error Check.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Redcap\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D1A661-8A5D-44BE-A064-A16428B26F4F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13830" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DHCPNDH1_DataDictionary_2019-08" sheetId="1" r:id="rId1"/>
@@ -17,12 +18,20 @@
     <sheet name="Variables" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21070" uniqueCount="3114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21049" uniqueCount="3114">
   <si>
     <t>Variable / Field Name</t>
   </si>
@@ -9403,7 +9412,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -10668,8 +10677,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:R1407" totalsRowShown="0">
-  <autoFilter ref="A1:R1407">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:R1407" totalsRowShown="0">
+  <autoFilter ref="A1:R1407" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="1">
       <filters>
         <filter val="scan_nursing_baby_info_today"/>
@@ -10677,32 +10686,32 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="18">
-    <tableColumn id="1" name="Variable / Field Name"/>
-    <tableColumn id="2" name="Form Name"/>
-    <tableColumn id="3" name="Section Header"/>
-    <tableColumn id="4" name="Field Type"/>
-    <tableColumn id="5" name="Field Label"/>
-    <tableColumn id="6" name="Choices, Calculations, OR Slider Labels"/>
-    <tableColumn id="7" name="Field Note"/>
-    <tableColumn id="8" name="Text Validation Type OR Show Slider Number"/>
-    <tableColumn id="9" name="Text Validation Min"/>
-    <tableColumn id="10" name="Text Validation Max"/>
-    <tableColumn id="11" name="Identifier?"/>
-    <tableColumn id="12" name="Branching Logic (Show field only if...)"/>
-    <tableColumn id="13" name="Required Field?"/>
-    <tableColumn id="14" name="Custom Alignment"/>
-    <tableColumn id="15" name="Question Number (surveys only)"/>
-    <tableColumn id="16" name="Matrix Group Name"/>
-    <tableColumn id="17" name="Matrix Ranking?"/>
-    <tableColumn id="18" name="Field Annotation"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Variable / Field Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Form Name"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Section Header"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Field Type"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Field Label"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Choices, Calculations, OR Slider Labels"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Field Note"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Text Validation Type OR Show Slider Number"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Text Validation Min"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Text Validation Max"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Identifier?"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Branching Logic (Show field only if...)"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Required Field?"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Custom Alignment"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Question Number (surveys only)"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Matrix Group Name"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Matrix Ranking?"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Field Annotation"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:T1407">
-  <autoFilter ref="A1:T1407">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table24" displayName="Table24" ref="A1:T1404">
+  <autoFilter ref="A1:T1404" xr:uid="{00000000-0009-0000-0100-000003000000}">
     <filterColumn colId="19">
       <filters>
         <filter val="No"/>
@@ -10710,54 +10719,54 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="20">
-    <tableColumn id="1" name="Variable / Field Name"/>
-    <tableColumn id="2" name="Form Name"/>
-    <tableColumn id="3" name="Section Header"/>
-    <tableColumn id="4" name="Field Type"/>
-    <tableColumn id="5" name="Field Label"/>
-    <tableColumn id="6" name="Choices, Calculations, OR Slider Labels" totalsRowDxfId="26"/>
-    <tableColumn id="7" name="Field Note"/>
-    <tableColumn id="8" name="Text Validation Type OR Show Slider Number"/>
-    <tableColumn id="9" name="Text Validation Min"/>
-    <tableColumn id="10" name="Text Validation Max"/>
-    <tableColumn id="11" name="Identifier?"/>
-    <tableColumn id="12" name="Branching Logic (Show field only if...)"/>
-    <tableColumn id="13" name="Required Field?"/>
-    <tableColumn id="14" name="Custom Alignment"/>
-    <tableColumn id="15" name="Question Number (surveys only)"/>
-    <tableColumn id="16" name="Matrix Group Name"/>
-    <tableColumn id="17" name="Matrix Ranking?"/>
-    <tableColumn id="18" name="Field Annotation" totalsRowFunction="count"/>
-    <tableColumn id="19" name="Black_List" dataDxfId="25"/>
-    <tableColumn id="22" name="Ignore" totalsRowFunction="count" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Variable / Field Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Form Name"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Section Header"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Field Type"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Field Label"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Choices, Calculations, OR Slider Labels" totalsRowDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Field Note"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Text Validation Type OR Show Slider Number"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Text Validation Min"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Text Validation Max"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Identifier?"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Branching Logic (Show field only if...)"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Required Field?"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Custom Alignment"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Question Number (surveys only)"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Matrix Group Name"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="Matrix Ranking?"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Field Annotation" totalsRowFunction="count"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="Black_List" dataDxfId="25"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="Ignore" totalsRowFunction="count" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:S197" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20" totalsRowBorderDxfId="19">
-  <autoFilter ref="A1:S197"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="A1:S197" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20" totalsRowBorderDxfId="19">
+  <autoFilter ref="A1:S197" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="19">
-    <tableColumn id="1" name="Variable / Field Name" dataDxfId="18"/>
-    <tableColumn id="2" name="Form Name" dataDxfId="17"/>
-    <tableColumn id="3" name="Section Header" dataDxfId="16"/>
-    <tableColumn id="4" name="Field Type" dataDxfId="15"/>
-    <tableColumn id="5" name="Field Label" dataDxfId="14"/>
-    <tableColumn id="6" name="Choices, Calculations, OR Slider Labels" dataDxfId="13"/>
-    <tableColumn id="7" name="Field Note" dataDxfId="12"/>
-    <tableColumn id="8" name="Text Validation Type OR Show Slider Number" dataDxfId="11"/>
-    <tableColumn id="9" name="Text Validation Min" dataDxfId="10"/>
-    <tableColumn id="10" name="Text Validation Max" dataDxfId="9"/>
-    <tableColumn id="11" name="Identifier?" dataDxfId="8"/>
-    <tableColumn id="12" name="Branching Logic (Show field only if...)" dataDxfId="7"/>
-    <tableColumn id="13" name="Required Field?" dataDxfId="6"/>
-    <tableColumn id="14" name="Custom Alignment" dataDxfId="5"/>
-    <tableColumn id="15" name="Question Number (surveys only)" dataDxfId="4"/>
-    <tableColumn id="16" name="Matrix Group Name" dataDxfId="3"/>
-    <tableColumn id="17" name="Matrix Ranking?" dataDxfId="2"/>
-    <tableColumn id="18" name="Field Annotation" dataDxfId="1"/>
-    <tableColumn id="19" name="Black_List" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Variable / Field Name" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Form Name" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Section Header" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Field Type" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Field Label" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Choices, Calculations, OR Slider Labels" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Field Note" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Text Validation Type OR Show Slider Number" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Text Validation Min" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Text Validation Max" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Identifier?" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Branching Logic (Show field only if...)" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Required Field?" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Custom Alignment" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Question Number (surveys only)" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Matrix Group Name" dataDxfId="3"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="Matrix Ranking?" dataDxfId="2"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="Field Annotation" dataDxfId="1"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0200-000013000000}" name="Black_List" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -11025,7 +11034,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R1407"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -39752,14 +39761,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T1407"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:T1404"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomRight" activeCell="B1405" sqref="B1405"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -77186,75 +77195,6 @@
         <v>3111</v>
       </c>
     </row>
-    <row r="1405" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1405" t="s">
-        <v>3091</v>
-      </c>
-      <c r="B1405" t="s">
-        <v>3092</v>
-      </c>
-      <c r="D1405" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1405" t="s">
-        <v>3093</v>
-      </c>
-      <c r="F1405" s="1" t="s">
-        <v>3094</v>
-      </c>
-      <c r="S1405" t="s">
-        <v>3112</v>
-      </c>
-      <c r="T1405" t="s">
-        <v>3111</v>
-      </c>
-    </row>
-    <row r="1406" spans="1:20" ht="75" x14ac:dyDescent="0.25">
-      <c r="A1406" t="s">
-        <v>3095</v>
-      </c>
-      <c r="B1406" t="s">
-        <v>3092</v>
-      </c>
-      <c r="D1406" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1406" t="s">
-        <v>3096</v>
-      </c>
-      <c r="F1406" s="1" t="s">
-        <v>3097</v>
-      </c>
-      <c r="L1406" t="s">
-        <v>3098</v>
-      </c>
-      <c r="S1406" t="s">
-        <v>3112</v>
-      </c>
-      <c r="T1406" t="s">
-        <v>3111</v>
-      </c>
-    </row>
-    <row r="1407" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1407" t="s">
-        <v>3099</v>
-      </c>
-      <c r="B1407" t="s">
-        <v>3092</v>
-      </c>
-      <c r="D1407" t="s">
-        <v>337</v>
-      </c>
-      <c r="E1407" t="s">
-        <v>3100</v>
-      </c>
-      <c r="S1407" t="s">
-        <v>3112</v>
-      </c>
-      <c r="T1407" t="s">
-        <v>3111</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -77264,7 +77204,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S197"/>
   <sheetViews>
     <sheetView topLeftCell="A174" workbookViewId="0">
@@ -83950,7 +83890,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="F4:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>